<commit_message>
Atualização Planilha de riscos
</commit_message>
<xml_diff>
--- a/Gestão/PlanilhadeRiscos Turtle life.xlsx
+++ b/Gestão/PlanilhadeRiscos Turtle life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\PRIMEIRO SEMESTRE\Pesquisa e Inovação\Sprint-2-turtlelife\Gestão\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02404236-CBCF-4097-9198-7F1DA96180E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A945F3-D21F-4B84-AA86-D9219437CE8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,14 +163,6 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -180,6 +172,14 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -201,25 +201,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -326,70 +326,76 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,6 +403,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -673,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C93DE82-BCFC-4C09-8298-3E550D735951}">
   <dimension ref="B2:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12:M12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,111 +704,111 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21" t="s">
+    <row r="6" spans="2:14" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="15" t="s">
+      <c r="H6" s="17"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="4"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="11"/>
     </row>
     <row r="7" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="12" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="11">
-        <v>3</v>
-      </c>
-      <c r="L7" s="10">
+      <c r="K7" s="23">
+        <v>3</v>
+      </c>
+      <c r="L7" s="12">
         <v>6</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="12">
         <v>9</v>
       </c>
-      <c r="N7" s="4"/>
+      <c r="N7" s="11"/>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="4"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="11"/>
     </row>
     <row r="9" spans="2:14" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
@@ -806,35 +817,35 @@
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="26">
         <v>1</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="26">
         <v>2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="25">
         <v>2</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="13" t="s">
+      <c r="I9" s="13"/>
+      <c r="J9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="25">
         <v>2</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="24">
         <v>4</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="6">
         <v>6</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="11"/>
     </row>
     <row r="10" spans="2:14" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
@@ -843,35 +854,35 @@
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="26">
         <v>1</v>
       </c>
-      <c r="E10" s="3">
-        <v>3</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="E10" s="26">
+        <v>3</v>
+      </c>
+      <c r="F10" s="24">
         <v>3</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="13" t="s">
+      <c r="I10" s="13"/>
+      <c r="J10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="25">
         <v>1</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="25">
         <v>2</v>
       </c>
-      <c r="M10" s="7">
-        <v>3</v>
-      </c>
-      <c r="N10" s="4"/>
+      <c r="M10" s="24">
+        <v>3</v>
+      </c>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" spans="2:14" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
@@ -880,33 +891,33 @@
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="26">
         <v>1</v>
       </c>
-      <c r="E11" s="3">
-        <v>3</v>
-      </c>
-      <c r="F11" s="3">
+      <c r="E11" s="26">
+        <v>3</v>
+      </c>
+      <c r="F11" s="24">
         <v>3</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6" t="s">
+      <c r="I11" s="13"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="M11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="4"/>
+      <c r="N11" s="11"/>
     </row>
     <row r="12" spans="2:14" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
@@ -915,29 +926,29 @@
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="26">
         <v>2</v>
       </c>
-      <c r="E12" s="3">
-        <v>3</v>
-      </c>
-      <c r="F12" s="3">
+      <c r="E12" s="26">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7">
         <v>6</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="14" t="s">
+      <c r="I12" s="13"/>
+      <c r="J12" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="4"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13" spans="2:14" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
@@ -946,19 +957,19 @@
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="26">
         <v>2</v>
       </c>
-      <c r="E13" s="3">
-        <v>3</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="E13" s="26">
+        <v>3</v>
+      </c>
+      <c r="F13" s="7">
         <v>6</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -969,19 +980,19 @@
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="26">
         <v>1</v>
       </c>
-      <c r="E14" s="3">
-        <v>3</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="E14" s="26">
+        <v>3</v>
+      </c>
+      <c r="F14" s="24">
         <v>3</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -992,29 +1003,24 @@
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="26">
         <v>1</v>
       </c>
-      <c r="E15" s="3">
-        <v>3</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="E15" s="26">
+        <v>3</v>
+      </c>
+      <c r="F15" s="24">
         <v>3</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="9" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="I6:I12"/>
     <mergeCell ref="N6:N12"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="B5:B8"/>
@@ -1023,6 +1029,11 @@
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="I6:I12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>